<commit_message>
graphique vitesse programme fini
</commit_message>
<xml_diff>
--- a/temps.xlsx
+++ b/temps.xlsx
@@ -380,6 +380,24 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1558,7 +1576,7 @@
   <dimension ref="B1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,6 +1644,9 @@
       <c r="D5">
         <v>50</v>
       </c>
+      <c r="E5">
+        <v>81</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6">
@@ -1637,6 +1658,9 @@
       <c r="D6">
         <v>49</v>
       </c>
+      <c r="E6">
+        <v>73</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7">
@@ -1648,6 +1672,9 @@
       <c r="D7">
         <v>54</v>
       </c>
+      <c r="E7">
+        <v>70</v>
+      </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -1659,6 +1686,9 @@
       <c r="D8">
         <v>52</v>
       </c>
+      <c r="E8">
+        <v>71</v>
+      </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9">
@@ -1670,6 +1700,9 @@
       <c r="D9">
         <v>43</v>
       </c>
+      <c r="E9">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -1680,6 +1713,9 @@
       </c>
       <c r="D10">
         <v>55</v>
+      </c>
+      <c r="E10">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>